<commit_message>
Dhaka City Total Added
</commit_message>
<xml_diff>
--- a/source-xlsx/12-04-2020.xlsx
+++ b/source-xlsx/12-04-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\covid19\source-xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711F54BA-CBA6-41BF-B7B9-A0D8ADC981E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380E7C98-AB76-4C6D-8182-E9DF71050B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="123">
   <si>
     <t>division</t>
   </si>
@@ -396,13 +396,19 @@
   </si>
   <si>
     <t xml:space="preserve">Wari </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhaka City </t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,16 +417,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri-Bold"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -443,17 +449,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -736,13 +738,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
@@ -751,21 +753,21 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -775,9 +777,8 @@
       <c r="C2" s="2">
         <v>22</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -787,9 +788,8 @@
       <c r="C3" s="2">
         <v>23</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -799,9 +799,8 @@
       <c r="C4" s="2">
         <v>10</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -811,9 +810,8 @@
       <c r="C5" s="2">
         <v>19</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -823,9 +821,8 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -835,9 +832,8 @@
       <c r="C7" s="2">
         <v>107</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -847,9 +843,8 @@
       <c r="C8" s="2">
         <v>14</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -859,9 +854,8 @@
       <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -871,9 +865,8 @@
       <c r="C10" s="2">
         <v>6</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -883,9 +876,8 @@
       <c r="C11" s="2">
         <v>2</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -895,9 +887,8 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -907,9 +898,8 @@
       <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -919,9 +909,8 @@
       <c r="C14" s="2">
         <v>12</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -931,9 +920,8 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -943,9 +931,8 @@
       <c r="C16" s="2">
         <v>9</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -955,9 +942,8 @@
       <c r="C17" s="2">
         <v>6</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -967,9 +953,8 @@
       <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -979,9 +964,8 @@
       <c r="C19" s="2">
         <v>6</v>
       </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -991,9 +975,8 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1003,9 +986,8 @@
       <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1015,9 +997,8 @@
       <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1027,9 +1008,8 @@
       <c r="C23" s="2">
         <v>2</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1039,9 +1019,8 @@
       <c r="C24" s="2">
         <v>6</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1051,9 +1030,8 @@
       <c r="C25" s="2">
         <v>3</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1063,9 +1041,8 @@
       <c r="C26" s="2">
         <v>1</v>
       </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -1075,9 +1052,8 @@
       <c r="C27" s="2">
         <v>3</v>
       </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1087,9 +1063,8 @@
       <c r="C28" s="2">
         <v>1</v>
       </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -1099,9 +1074,8 @@
       <c r="C29" s="2">
         <v>5</v>
       </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -1111,9 +1085,8 @@
       <c r="C30" s="2">
         <v>6</v>
       </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1123,9 +1096,8 @@
       <c r="C31" s="2">
         <v>1</v>
       </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1135,9 +1107,8 @@
       <c r="C32" s="2">
         <v>2</v>
       </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1147,9 +1118,8 @@
       <c r="C33" s="2">
         <v>3</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -1159,9 +1129,8 @@
       <c r="C34" s="2">
         <v>1</v>
       </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -1171,10 +1140,9 @@
       <c r="C35" s="2">
         <v>3</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="5" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1187,8 +1155,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1201,8 +1169,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1215,8 +1183,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1229,8 +1197,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -1243,8 +1211,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -1257,8 +1225,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -1271,8 +1239,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1285,8 +1253,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -1299,8 +1267,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -1313,8 +1281,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -1327,8 +1295,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -1341,8 +1309,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -1355,8 +1323,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -1369,8 +1337,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -1383,8 +1351,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -1397,8 +1365,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -1411,8 +1379,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -1425,8 +1393,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="5" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -1439,8 +1407,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="5" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -1453,8 +1421,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="5" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -1467,8 +1435,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -1481,8 +1449,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -1495,8 +1463,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="5" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -1509,8 +1477,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="5" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -1523,8 +1491,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="5" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -1537,8 +1505,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -1551,8 +1519,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="5" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -1565,8 +1533,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="5" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -1579,8 +1547,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="5" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -1593,8 +1561,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -1607,8 +1575,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="5" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -1621,8 +1589,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -1635,8 +1603,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="5" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -1649,8 +1617,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="5" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -1663,8 +1631,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="5" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -1677,8 +1645,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="5" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -1691,8 +1659,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="5" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -1705,8 +1673,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="5" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -1719,8 +1687,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="5" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -1733,8 +1701,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="5" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -1747,8 +1715,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="5" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -1761,8 +1729,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="5" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -1775,8 +1743,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="5" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -1789,8 +1757,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="5" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -1803,8 +1771,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="5" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -1817,8 +1785,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="5" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -1831,8 +1799,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="5" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -1845,8 +1813,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="5" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -1859,8 +1827,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="5" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -1873,8 +1841,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="5" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -1887,8 +1855,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="5" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -1901,8 +1869,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="5" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -1915,8 +1883,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="5" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -1929,8 +1897,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="5" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -1943,8 +1911,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="5" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -1957,8 +1925,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="5" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -1971,8 +1939,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="5" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -1985,8 +1953,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="5" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -1999,8 +1967,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="5" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -2013,8 +1981,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="5" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -2027,8 +1995,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="5" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -2041,8 +2009,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="5" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -2055,8 +2023,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="5" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -2069,8 +2037,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="5" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -2083,8 +2051,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="5" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -2097,8 +2065,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="5" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -2111,8 +2079,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="5" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -2125,8 +2093,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="5" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -2139,8 +2107,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="5" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -2153,8 +2121,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="5" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -2167,8 +2135,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="5" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -2181,8 +2149,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="5" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -2195,8 +2163,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="5" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -2209,8 +2177,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="5" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -2223,257 +2191,19 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="3:4">
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="3:4">
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="3:4">
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="3:4">
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="3:4">
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="3:4">
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="3:4">
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="3:4">
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="3:4">
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="3:4">
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="3:4">
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-    </row>
-    <row r="124" spans="3:4">
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-    </row>
-    <row r="125" spans="3:4">
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-    </row>
-    <row r="126" spans="3:4">
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-    </row>
-    <row r="127" spans="3:4">
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-    </row>
-    <row r="128" spans="3:4">
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="3:4">
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="3:4">
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="3:4">
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-    </row>
-    <row r="132" spans="3:4">
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-    </row>
-    <row r="133" spans="3:4">
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-    </row>
-    <row r="134" spans="3:4">
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-    </row>
-    <row r="135" spans="3:4">
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-    </row>
-    <row r="136" spans="3:4">
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-    </row>
-    <row r="137" spans="3:4">
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-    </row>
-    <row r="138" spans="3:4">
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-    </row>
-    <row r="139" spans="3:4">
-      <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-    </row>
-    <row r="140" spans="3:4">
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-    </row>
-    <row r="141" spans="3:4">
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-    </row>
-    <row r="142" spans="3:4">
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-    </row>
-    <row r="143" spans="3:4">
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-    </row>
-    <row r="144" spans="3:4">
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-    </row>
-    <row r="145" spans="3:4">
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-    </row>
-    <row r="146" spans="3:4">
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-    </row>
-    <row r="147" spans="3:4">
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-    </row>
-    <row r="148" spans="3:4">
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-    </row>
-    <row r="149" spans="3:4">
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-    </row>
-    <row r="150" spans="3:4">
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-    </row>
-    <row r="151" spans="3:4">
-      <c r="C151" s="3"/>
-      <c r="D151" s="2"/>
-    </row>
-    <row r="152" spans="3:4">
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-    </row>
-    <row r="153" spans="3:4">
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-    </row>
-    <row r="154" spans="3:4">
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-    </row>
-    <row r="155" spans="3:4">
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-    </row>
-    <row r="156" spans="3:4">
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-    </row>
-    <row r="157" spans="3:4">
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-    </row>
-    <row r="158" spans="3:4">
-      <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
-    </row>
-    <row r="159" spans="3:4">
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-    </row>
-    <row r="160" spans="3:4">
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-    </row>
-    <row r="161" spans="3:4">
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
-    </row>
-    <row r="162" spans="3:4">
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-    </row>
-    <row r="163" spans="3:4">
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
-    </row>
-    <row r="164" spans="3:4">
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
-    </row>
-    <row r="165" spans="3:4">
-      <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
-    </row>
-    <row r="166" spans="3:4">
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-    </row>
-    <row r="167" spans="3:4">
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-    </row>
-    <row r="168" spans="3:4">
-      <c r="C168" s="2"/>
-      <c r="D168" s="2"/>
-    </row>
-    <row r="169" spans="3:4">
-      <c r="C169" s="2"/>
-      <c r="D169" s="2"/>
-    </row>
-    <row r="170" spans="3:4">
-      <c r="C170" s="2"/>
-      <c r="D170" s="2"/>
-    </row>
-    <row r="171" spans="3:4">
-      <c r="C171" s="2"/>
-      <c r="D171" s="2"/>
-    </row>
-    <row r="172" spans="3:4">
-      <c r="C172" s="2"/>
-      <c r="D172" s="2"/>
-    </row>
-    <row r="173" spans="3:4">
-      <c r="C173" s="2"/>
-      <c r="D173" s="2"/>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" s="2">
+        <v>313</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>